<commit_message>
add function to read txt and csv file
</commit_message>
<xml_diff>
--- a/data/drive.ecepvn.org/sinhvien_sang_nhom13.xlsx
+++ b/data/drive.ecepvn.org/sinhvien_sang_nhom13.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\workspace\atSchool\2019-2020-HK2\DataWarehouse\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\workspace\school\2019-2020-HK2\DataWarehouse\data\sinhvien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DEA5D8-A4B5-44AD-9822-33B3F6A00E0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863A5CCD-3FE3-44AD-813C-9F21872F7479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="537">
   <si>
     <t>firstname</t>
   </si>
@@ -1636,6 +1636,9 @@
   </si>
   <si>
     <t>17125372@st.hcmuaf.edu.vn</t>
+  </si>
+  <si>
+    <t>note</t>
   </si>
 </sst>
 </file>
@@ -2505,10 +2508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1000"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2527,7 +2530,7 @@
     <col min="30" max="16384" width="12.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>49</v>
       </c>
@@ -2561,8 +2564,11 @@
       <c r="K1" s="23" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>95</v>
       </c>
@@ -2597,7 +2603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>97</v>
       </c>
@@ -2632,7 +2638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>99</v>
       </c>
@@ -2667,7 +2673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>101</v>
       </c>
@@ -2702,7 +2708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>103</v>
       </c>
@@ -2737,7 +2743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>105</v>
       </c>
@@ -2772,7 +2778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>107</v>
       </c>
@@ -2807,7 +2813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>109</v>
       </c>
@@ -2842,7 +2848,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>111</v>
       </c>
@@ -2877,7 +2883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>113</v>
       </c>
@@ -2912,7 +2918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>115</v>
       </c>
@@ -2947,7 +2953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>117</v>
       </c>
@@ -2982,7 +2988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>119</v>
       </c>
@@ -3017,7 +3023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>121</v>
       </c>
@@ -3052,7 +3058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>123</v>
       </c>

</xml_diff>